<commit_message>
Refactor VBA code for importing and processing data
</commit_message>
<xml_diff>
--- a/data/A envoyer_antoine(non corrompue)/A envoyer/Plateaux_Exp.xlsx
+++ b/data/A envoyer_antoine(non corrompue)/A envoyer/Plateaux_Exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\travail\stage et4\travail\codePlateau\data\A envoyer_antoine(non corrompue)\A envoyer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C9B091-A520-4521-A84C-587E9E16D84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20640AFA-3BA7-40DC-BC09-739169AD4090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,7 +759,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changement de paradigme fonctionne
</commit_message>
<xml_diff>
--- a/data/A envoyer_antoine(non corrompue)/A envoyer/Plateaux_Exp.xlsx
+++ b/data/A envoyer_antoine(non corrompue)/A envoyer/Plateaux_Exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\travail\stage et4\travail\codePlateau\data\A envoyer_antoine(non corrompue)\A envoyer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D3E3F8-33CE-4452-B04F-A461B031850D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191790D4-08AB-44ED-8724-31CBCA9903FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,7 +759,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>